<commit_message>
all nighter of work
</commit_message>
<xml_diff>
--- a/PowerGridResearch/Code/DCPF-MST/data.xlsx
+++ b/PowerGridResearch/Code/DCPF-MST/data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian French\Documents\GitHub\PowerGridResearch\PowerGridResearch\Code\DCPF-MST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8362DCA6-2CD0-45FF-B251-8B4CAAD8DD6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7AB482-EA4D-4C71-8728-1E1AAFF8AFA6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
   </bookViews>
   <sheets>
     <sheet name="GeoScenario" sheetId="1" r:id="rId1"/>
+    <sheet name="Bus 57 Random-No Limits" sheetId="2" r:id="rId2"/>
+    <sheet name="Bus57--With Limits" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>timestep</t>
   </si>
@@ -52,6 +54,12 @@
   </si>
   <si>
     <t>Summed</t>
+  </si>
+  <si>
+    <t>Nominal Roads</t>
+  </si>
+  <si>
+    <t>No Travel Times</t>
   </si>
 </sst>
 </file>
@@ -1391,6 +1399,503 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Shift by Shift losses</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> on IEEE Bus 57 without line limits</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus 57 Random-No Limits'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RoadFirst</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus 57 Random-No Limits'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>543.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159.29999999999899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113.299999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5884-451B-83C5-F609D034D194}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus 57 Random-No Limits'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nominal Roads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus 57 Random-No Limits'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>543.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>543.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159.29999999999899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5884-451B-83C5-F609D034D194}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus 57 Random-No Limits'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Travel Times</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus 57 Random-No Limits'!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>543.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159.29999999999899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113.299999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5884-451B-83C5-F609D034D194}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="557275888"/>
+        <c:axId val="557276544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="557275888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="557276544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="557276544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="557275888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1471,6 +1976,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1975,6 +2520,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2546,6 +3594,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E0D1377-8810-481F-B0EC-9B9F7F93A916}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2853,8 +3942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FEBF82-81C8-4A41-8184-BAB1DED90955}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3187,4 +4276,451 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8676E6-EE69-4DEF-ADC7-ED125A051ED3}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>543.1</v>
+      </c>
+      <c r="C2">
+        <v>543.1</v>
+      </c>
+      <c r="D2">
+        <v>543.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>159.29999999999899</v>
+      </c>
+      <c r="C3">
+        <v>543.1</v>
+      </c>
+      <c r="D3">
+        <v>159.29999999999899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>113.299999999999</v>
+      </c>
+      <c r="C4">
+        <v>159.29999999999899</v>
+      </c>
+      <c r="D4">
+        <v>113.299999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>91.3</v>
+      </c>
+      <c r="C5">
+        <v>113.299999999999</v>
+      </c>
+      <c r="D5">
+        <v>91.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>88.6</v>
+      </c>
+      <c r="C6">
+        <v>91.3</v>
+      </c>
+      <c r="D6">
+        <v>91.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>88.6</v>
+      </c>
+      <c r="C7">
+        <v>88.3</v>
+      </c>
+      <c r="D7">
+        <v>87.299999999999898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2)</f>
+        <v>543.1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="0">SUM(C2)</f>
+        <v>543.1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>543.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B2:B3)</f>
+        <v>702.39999999999895</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="1">SUM(C2:C3)</f>
+        <v>1086.2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>702.39999999999895</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B2:B4)</f>
+        <v>815.699999999998</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="2">SUM(C2:C4)</f>
+        <v>1245.4999999999991</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>815.699999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B5)</f>
+        <v>906.99999999999795</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:D14" si="3">SUM(C2:C5)</f>
+        <v>1358.7999999999981</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>906.99999999999795</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B2:B6)</f>
+        <v>995.59999999999798</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:D15" si="4">SUM(C2:C6)</f>
+        <v>1450.0999999999981</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="4"/>
+        <v>998.29999999999791</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <f>SUM(B2:B7)</f>
+        <v>1084.199999999998</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="5">SUM(C2:C7)</f>
+        <v>1538.399999999998</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="5"/>
+        <v>1085.5999999999979</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8219BB0E-3807-45E0-A80F-E0B818C19BC8}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>517.1</v>
+      </c>
+      <c r="C2">
+        <v>517.1</v>
+      </c>
+      <c r="D2">
+        <v>517.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>133.29999999999899</v>
+      </c>
+      <c r="C3">
+        <v>133.29999999999899</v>
+      </c>
+      <c r="D3">
+        <v>133.29999999999899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>87.299999999999898</v>
+      </c>
+      <c r="C4">
+        <v>87.299999999999898</v>
+      </c>
+      <c r="D4">
+        <v>87.299999999999898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>84.299999999999898</v>
+      </c>
+      <c r="C5">
+        <v>83.699999999999903</v>
+      </c>
+      <c r="D5">
+        <v>65.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>83.699999999999903</v>
+      </c>
+      <c r="C6">
+        <v>83.699999999999903</v>
+      </c>
+      <c r="D6">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>83.8</v>
+      </c>
+      <c r="C7">
+        <v>83.6</v>
+      </c>
+      <c r="D7">
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2)</f>
+        <v>517.1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="0">SUM(C2)</f>
+        <v>517.1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>517.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B2:B3)</f>
+        <v>650.39999999999895</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="1">SUM(C2:C3)</f>
+        <v>650.39999999999895</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>650.39999999999895</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B2:B4)</f>
+        <v>737.69999999999891</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="2">SUM(C2:C4)</f>
+        <v>737.69999999999891</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>737.69999999999891</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B5)</f>
+        <v>821.99999999999886</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:D14" si="3">SUM(C2:C5)</f>
+        <v>821.39999999999884</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>802.99999999999886</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B2:B6)</f>
+        <v>905.69999999999879</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:D15" si="4">SUM(C2:C6)</f>
+        <v>905.09999999999877</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="4"/>
+        <v>855.29999999999882</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <f>SUM(B2:B7)</f>
+        <v>989.49999999999875</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="5">SUM(C2:C7)</f>
+        <v>988.69999999999879</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="5"/>
+        <v>902.59999999999877</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
paper stuff and code fixes
</commit_message>
<xml_diff>
--- a/PowerGridResearch/Code/DCPF-MST/data.xlsx
+++ b/PowerGridResearch/Code/DCPF-MST/data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian French\Documents\GitHub\PowerGridResearch\PowerGridResearch\Code\DCPF-MST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36355AC7-2576-40A2-8133-0FC307096F3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1B5C1F-66C4-4E04-AAC8-AA6F1503A1B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
   </bookViews>
   <sheets>
-    <sheet name="GeoScenario" sheetId="1" r:id="rId1"/>
+    <sheet name="Bus 30" sheetId="1" r:id="rId1"/>
     <sheet name="Bus57--With Limits" sheetId="3" r:id="rId2"/>
+    <sheet name="Bus 30 Scenario 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,24 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>timestep</t>
-  </si>
-  <si>
-    <t>RoadFirst</t>
-  </si>
-  <si>
-    <t>Damaged Roads</t>
-  </si>
-  <si>
-    <t>Repaired Roads</t>
-  </si>
-  <si>
-    <t>Pure Schedule</t>
-  </si>
-  <si>
-    <t>PostProcessed Schedule</t>
   </si>
   <si>
     <t>Summed</t>
@@ -58,13 +45,43 @@
     <t>Nominal Roads</t>
   </si>
   <si>
-    <t>No Travel Times</t>
+    <t>Post Processed with Nominal Roads</t>
   </si>
   <si>
-    <t>Post Processed Nominal</t>
+    <t>No Travel Times Pure Scheduling</t>
   </si>
   <si>
-    <t>Post Processed Damaged</t>
+    <t>Power Repair Conditioned on Road Repair</t>
+  </si>
+  <si>
+    <t>Statically Samaged Roads</t>
+  </si>
+  <si>
+    <t>Power Repair with Nominal Roads</t>
+  </si>
+  <si>
+    <t>No Travel Time Pure Schedule</t>
+  </si>
+  <si>
+    <t>PostProcessed Schedule with Nominal Roads</t>
+  </si>
+  <si>
+    <t>damaged Roads</t>
+  </si>
+  <si>
+    <t>Power Repair Conditional on Road Repair</t>
+  </si>
+  <si>
+    <t>Discrete</t>
+  </si>
+  <si>
+    <t>Continuous w/o node flow</t>
+  </si>
+  <si>
+    <t>Continuous w/ node flow limits</t>
+  </si>
+  <si>
+    <t>tightened line limits</t>
   </si>
 </sst>
 </file>
@@ -156,6 +173,11 @@
               <a:rPr lang="en-US"/>
               <a:t>Load Shed by Step</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in the 30 Bus Case</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -199,11 +221,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$B$1</c:f>
+              <c:f>'Bus 30'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RoadFirst</c:v>
+                  <c:v>Power Repair Conditioned on Road Repair</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -234,7 +256,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$B$2:$B$8</c:f>
+              <c:f>'Bus 30'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -271,11 +293,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$C$1</c:f>
+              <c:f>'Bus 30'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Damaged Roads</c:v>
+                  <c:v>Statically Samaged Roads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -306,7 +328,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$C$2:$C$8</c:f>
+              <c:f>'Bus 30'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -343,11 +365,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$D$1</c:f>
+              <c:f>'Bus 30'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Repaired Roads</c:v>
+                  <c:v>Power Repair with Nominal Roads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -378,7 +400,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$D$2:$D$8</c:f>
+              <c:f>'Bus 30'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -418,11 +440,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$E$1</c:f>
+              <c:f>'Bus 30'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pure Schedule</c:v>
+                  <c:v>No Travel Time Pure Schedule</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -453,7 +475,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$E$2:$E$8</c:f>
+              <c:f>'Bus 30'!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -490,11 +512,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$F$1</c:f>
+              <c:f>'Bus 30'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PostProcessed Schedule</c:v>
+                  <c:v>PostProcessed Schedule with Nominal Roads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -525,7 +547,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$F$2:$F$8</c:f>
+              <c:f>'Bus 30'!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -580,6 +602,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Shift Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -644,6 +721,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MW of Load Shed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -847,11 +979,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$B$1</c:f>
+              <c:f>'Bus 30'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RoadFirst</c:v>
+                  <c:v>Power Repair Conditioned on Road Repair</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -882,7 +1014,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$B$11:$B$16</c:f>
+              <c:f>'Bus 30'!$B$11:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -919,11 +1051,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$C$1</c:f>
+              <c:f>'Bus 30'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Damaged Roads</c:v>
+                  <c:v>Statically Samaged Roads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -954,7 +1086,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$C$11:$C$16</c:f>
+              <c:f>'Bus 30'!$C$11:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -991,11 +1123,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$D$1</c:f>
+              <c:f>'Bus 30'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Repaired Roads</c:v>
+                  <c:v>Power Repair with Nominal Roads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1026,7 +1158,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$D$11:$D$16</c:f>
+              <c:f>'Bus 30'!$D$11:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1063,11 +1195,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$E$1</c:f>
+              <c:f>'Bus 30'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pure Schedule</c:v>
+                  <c:v>No Travel Time Pure Schedule</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1098,7 +1230,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$E$11:$E$16</c:f>
+              <c:f>'Bus 30'!$E$11:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1135,11 +1267,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>GeoScenario!$F$1</c:f>
+              <c:f>'Bus 30'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PostProcessed Schedule</c:v>
+                  <c:v>PostProcessed Schedule with Nominal Roads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1170,7 +1302,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GeoScenario!$F$11:$F$16</c:f>
+              <c:f>'Bus 30'!$F$11:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1404,6 +1536,1854 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power Repair Conditional on Road Repair</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADEE-4F11-BD5F-B460814AC71F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Travel Times Pure Scheduling</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>133.29999999999899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.799999999999901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ADEE-4F11-BD5F-B460814AC71F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Post Processed with Nominal Roads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>133.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-ADEE-4F11-BD5F-B460814AC71F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="554326544"/>
+        <c:axId val="562441752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="554326544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562441752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="562441752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554326544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Loss</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> over time on the 57 Bus Case</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power Repair Conditional on Road Repair</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADEE-4F11-BD5F-B460814AC71F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nominal Roads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>133.29999999999899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111.399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ADEE-4F11-BD5F-B460814AC71F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Travel Times Pure Scheduling</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>133.29999999999899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.799999999999901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-ADEE-4F11-BD5F-B460814AC71F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Post Processed with Nominal Roads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>133.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F4D3-4CBC-B9D1-89456EABB673}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bus57--With Limits'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>damaged Roads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>517.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118.19999999999899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6019-48EF-BDBA-654E0B11B337}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="554326544"/>
+        <c:axId val="562441752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="554326544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Shift</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Number</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562441752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="562441752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MW</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Demand Shed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554326544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$A$4:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D2D2-43EB-BE49-8473906F9A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>118.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D2D2-43EB-BE49-8473906F9A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>111.399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D2D2-43EB-BE49-8473906F9A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D2D2-43EB-BE49-8473906F9A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>133.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D2D2-43EB-BE49-8473906F9A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bus57--With Limits'!$F$4:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>118.19999999999899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.299999999999898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D2D2-43EB-BE49-8473906F9A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="549520152"/>
+        <c:axId val="549520808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="549520152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549520808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="549520808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549520152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1484,6 +3464,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2490,20 +4590,1529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1419225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2530,16 +6139,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>461962</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>157162</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2559,6 +6168,119 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBDD6C88-B638-4A81-B577-8A9E68604FD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>436562</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7196844-2444-4C21-8267-1EBC764F765F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2028825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1956CACA-1FFD-4A71-9079-83CE8F772D8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2864,18 +6586,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FEBF82-81C8-4A41-8184-BAB1DED90955}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B16"/>
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2883,19 +6606,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3028,12 +6751,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F9">
-        <v>0</v>
+        <f>SUM(F2:F8)</f>
+        <v>420.2000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3186,7 +6910,7 @@
         <v>409.60000000000008</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D2:D8)</f>
         <v>539.5</v>
@@ -3194,6 +6918,12 @@
       <c r="F17">
         <f>SUM(F2:F8)</f>
         <v>420.2000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f>B16/E16</f>
+        <v>1.0356108859293571</v>
       </c>
     </row>
   </sheetData>
@@ -3204,14 +6934,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8219BB0E-3807-45E0-A80F-E0B818C19BC8}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
@@ -3222,16 +6953,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
@@ -3241,10 +6972,19 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>517.1</v>
+      </c>
+      <c r="C2">
+        <v>517.1</v>
+      </c>
       <c r="D2">
         <v>517.1</v>
       </c>
       <c r="E2">
+        <v>517.1</v>
+      </c>
+      <c r="F2">
         <v>517.1</v>
       </c>
     </row>
@@ -3252,10 +6992,19 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>140.1</v>
+      </c>
+      <c r="C3">
+        <v>133.29999999999899</v>
+      </c>
       <c r="D3">
         <v>133.29999999999899</v>
       </c>
       <c r="E3">
+        <v>140.1</v>
+      </c>
+      <c r="F3">
         <v>140.1</v>
       </c>
     </row>
@@ -3263,43 +7012,79 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>118.1</v>
+      </c>
+      <c r="C4">
+        <v>111.399999999999</v>
+      </c>
       <c r="D4">
         <v>87.299999999999898</v>
       </c>
       <c r="E4">
         <v>133.30000000000001</v>
+      </c>
+      <c r="F4">
+        <v>118.19999999999899</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>96.2</v>
+      </c>
+      <c r="C5">
+        <v>87.299999999999898</v>
+      </c>
       <c r="D5">
         <v>65.3</v>
       </c>
       <c r="E5">
         <v>87.3</v>
+      </c>
+      <c r="F5">
+        <v>96.2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>65.3</v>
+      </c>
+      <c r="C6">
+        <v>65.3</v>
+      </c>
       <c r="D6">
         <v>65.3</v>
       </c>
       <c r="E6">
         <v>65.3</v>
+      </c>
+      <c r="F6">
+        <v>87.299999999999898</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>65.3</v>
+      </c>
+      <c r="C7">
+        <v>52.3</v>
+      </c>
       <c r="D7">
         <v>38.799999999999997</v>
       </c>
       <c r="E7">
+        <v>65.3</v>
+      </c>
+      <c r="F7">
         <v>65.3</v>
       </c>
     </row>
@@ -3334,6 +7119,352 @@
       </c>
       <c r="E10">
         <v>24.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" ref="B11:E11" si="0">SUM(B2:B7)</f>
+        <v>1002.1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>966.69999999999777</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>907.09999999999877</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1008.3999999999999</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F2:F7)</f>
+        <v>1024.1999999999989</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B361CE4-9FB9-4968-BD88-72584EBD2BB8}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>221.69999999999899</v>
+      </c>
+      <c r="C2">
+        <v>221.69999999999899</v>
+      </c>
+      <c r="D2">
+        <v>221.7</v>
+      </c>
+      <c r="E2">
+        <v>221.69999999999899</v>
+      </c>
+      <c r="F2">
+        <v>221.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>104.7</v>
+      </c>
+      <c r="C3">
+        <v>104.7</v>
+      </c>
+      <c r="D3">
+        <v>221.69999999999899</v>
+      </c>
+      <c r="E3">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="F3">
+        <v>221.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>83.8</v>
+      </c>
+      <c r="C4">
+        <v>83.8</v>
+      </c>
+      <c r="D4">
+        <v>83.8</v>
+      </c>
+      <c r="E4">
+        <v>49.099999999999902</v>
+      </c>
+      <c r="F4">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>60.5</v>
+      </c>
+      <c r="C5">
+        <v>74.8</v>
+      </c>
+      <c r="D5">
+        <v>60.5</v>
+      </c>
+      <c r="E5">
+        <v>39.599999999999902</v>
+      </c>
+      <c r="F5">
+        <v>49.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>49.099999999999902</v>
+      </c>
+      <c r="C6">
+        <v>74.8</v>
+      </c>
+      <c r="D6">
+        <v>49.099999999999902</v>
+      </c>
+      <c r="E6">
+        <v>30.6</v>
+      </c>
+      <c r="F6">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>39.599999999999902</v>
+      </c>
+      <c r="C7">
+        <v>74.8</v>
+      </c>
+      <c r="D7">
+        <v>39.599999999999902</v>
+      </c>
+      <c r="E7">
+        <v>27.4</v>
+      </c>
+      <c r="F7">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>559.39999999999884</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="0">SUM(C2:C7)</f>
+        <v>634.599999999999</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v>676.39999999999873</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>443.99999999999881</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>635.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBE892F-7ACA-4E49-8EEA-B80ED9C43321}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>221.69999999999899</v>
+      </c>
+      <c r="C2">
+        <v>221.69999999999899</v>
+      </c>
+      <c r="D2">
+        <v>221.69999999999899</v>
+      </c>
+      <c r="E2">
+        <v>221.69999999999899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="C3">
+        <v>104.7</v>
+      </c>
+      <c r="D3">
+        <v>92.500003976943304</v>
+      </c>
+      <c r="E3">
+        <v>92.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="C4">
+        <v>83.8</v>
+      </c>
+      <c r="D4">
+        <v>83.799992687555701</v>
+      </c>
+      <c r="E4">
+        <v>83.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>34.999994945919099</v>
+      </c>
+      <c r="C5">
+        <v>60.5</v>
+      </c>
+      <c r="D5">
+        <v>60.499992687555697</v>
+      </c>
+      <c r="E5">
+        <v>60.499819331823701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>23.599998993564501</v>
+      </c>
+      <c r="C6">
+        <v>49.099999999999902</v>
+      </c>
+      <c r="D6">
+        <v>49.099994227017604</v>
+      </c>
+      <c r="E6">
+        <v>49.099999999999902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>14.899999052022</v>
+      </c>
+      <c r="C7">
+        <v>39.599999999999902</v>
+      </c>
+      <c r="D7">
+        <v>39.599994227017604</v>
+      </c>
+      <c r="E7">
+        <v>40.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resilience data and thesis updates
</commit_message>
<xml_diff>
--- a/PowerGridResearch/Code/DCPF-MST/data.xlsx
+++ b/PowerGridResearch/Code/DCPF-MST/data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian French\Documents\GitHub\PowerGridResearch\PowerGridResearch\Code\DCPF-MST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807BBE01-25BA-45E9-A9DF-A13076C44E8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D581272-2E38-4ACC-B591-18607A1EBA7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus 30" sheetId="1" r:id="rId1"/>
     <sheet name="Bus57--With Limits" sheetId="3" r:id="rId2"/>
     <sheet name="Bus 30 Scenario 2" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Resilience1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>timestep</t>
   </si>
@@ -100,6 +101,12 @@
   </si>
   <si>
     <t>Rand Case 3</t>
+  </si>
+  <si>
+    <t>"optimal" resilience for 1 node and 3 edges</t>
+  </si>
+  <si>
+    <t>Time Steps</t>
   </si>
 </sst>
 </file>
@@ -7209,7 +7216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B361CE4-9FB9-4968-BD88-72584EBD2BB8}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F27:F28"/>
     </sheetView>
   </sheetViews>
@@ -7690,4 +7697,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B5923C-FB1B-462C-A67F-839D1BF542D0}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>231.69999999999899</v>
+      </c>
+      <c r="C3">
+        <v>231.69999999999899</v>
+      </c>
+      <c r="D3">
+        <v>261.69999999999902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>104.7</v>
+      </c>
+      <c r="C4">
+        <v>93</v>
+      </c>
+      <c r="D4">
+        <v>134.69999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>35.4</v>
+      </c>
+      <c r="C5">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="D5">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>35.4</v>
+      </c>
+      <c r="C6">
+        <v>40.099999999999902</v>
+      </c>
+      <c r="D6">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>35.4</v>
+      </c>
+      <c r="C7">
+        <v>24.2</v>
+      </c>
+      <c r="D7">
+        <v>38.199999999999903</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>35.4</v>
+      </c>
+      <c r="C8">
+        <v>24.2</v>
+      </c>
+      <c r="D8">
+        <v>25.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data and writing updates for resilience
</commit_message>
<xml_diff>
--- a/PowerGridResearch/Code/DCPF-MST/data.xlsx
+++ b/PowerGridResearch/Code/DCPF-MST/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian French\Documents\GitHub\PowerGridResearch\PowerGridResearch\Code\DCPF-MST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D581272-2E38-4ACC-B591-18607A1EBA7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBC4B62-C83D-499A-AEEE-E57F01757641}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
+    <workbookView xWindow="34875" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus 30" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Bus 30 Scenario 2" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
     <sheet name="Resilience1" sheetId="6" r:id="rId5"/>
+    <sheet name="Resilience12" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>timestep</t>
   </si>
@@ -107,6 +108,15 @@
   </si>
   <si>
     <t>Time Steps</t>
+  </si>
+  <si>
+    <t>Random Resilience on same data</t>
+  </si>
+  <si>
+    <t>Optimal Resilience</t>
+  </si>
+  <si>
+    <t>Random Resilience</t>
   </si>
 </sst>
 </file>
@@ -7701,15 +7711,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B5923C-FB1B-462C-A67F-839D1BF542D0}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7721,80 +7731,515 @@
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>231.69999999999899</v>
       </c>
       <c r="C3">
-        <v>231.69999999999899</v>
+        <v>253.39999999999901</v>
       </c>
       <c r="D3">
-        <v>261.69999999999902</v>
+        <v>114.7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>104.7</v>
+        <v>124.1</v>
       </c>
       <c r="C4">
-        <v>93</v>
+        <v>129.9</v>
       </c>
       <c r="D4">
-        <v>134.69999999999999</v>
+        <v>53.099999999999902</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>35.4</v>
+        <v>18.7</v>
       </c>
       <c r="C5">
-        <v>75.099999999999994</v>
+        <v>129.9</v>
       </c>
       <c r="D5">
-        <v>93.7</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>35.4</v>
+        <v>15.2</v>
       </c>
       <c r="C6">
-        <v>40.099999999999902</v>
+        <v>124.1</v>
       </c>
       <c r="D6">
-        <v>63.7</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>35.4</v>
+        <v>15.2</v>
       </c>
       <c r="C7">
-        <v>24.2</v>
+        <v>124.1</v>
       </c>
       <c r="D7">
-        <v>38.199999999999903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>35.4</v>
+        <v>15.2</v>
       </c>
       <c r="C8">
-        <v>24.2</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>25.5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>231.69999999999899</v>
+      </c>
+      <c r="C11">
+        <v>253.39999999999901</v>
+      </c>
+      <c r="D11">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>124.1</v>
+      </c>
+      <c r="C12">
+        <v>253.39999999999901</v>
+      </c>
+      <c r="D12">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>16.3</v>
+      </c>
+      <c r="C13">
+        <v>253.39999999999901</v>
+      </c>
+      <c r="D13">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12.8</v>
+      </c>
+      <c r="C14">
+        <v>38.699999999999903</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12.8</v>
+      </c>
+      <c r="C15">
+        <v>2.4</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>12.8</v>
+      </c>
+      <c r="C16">
+        <v>2.4</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946CCB79-A94E-4848-8DCC-31F38FA0F6DB}">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>250.99999999999901</v>
+      </c>
+      <c r="C2">
+        <v>283.39999999999998</v>
+      </c>
+      <c r="D2">
+        <v>107.1</v>
+      </c>
+      <c r="E2">
+        <v>283.39999999999998</v>
+      </c>
+      <c r="F2">
+        <v>259.29999999999899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>55.8</v>
+      </c>
+      <c r="C3">
+        <v>137</v>
+      </c>
+      <c r="D3">
+        <v>37.6</v>
+      </c>
+      <c r="E3">
+        <v>99.2</v>
+      </c>
+      <c r="F3">
+        <v>73.599999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>14.1</v>
+      </c>
+      <c r="C4">
+        <v>84.2</v>
+      </c>
+      <c r="D4">
+        <v>22.4</v>
+      </c>
+      <c r="E4">
+        <v>60.5</v>
+      </c>
+      <c r="F4">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>39.599999999999902</v>
+      </c>
+      <c r="F5">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>26.299999999999901</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>18.7</v>
+      </c>
+      <c r="F6">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>12.8</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>SUM(A2:A8)</f>
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:Q9" si="0">SUM(B2:B8)</f>
+        <v>320.89999999999901</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>588.89999999999986</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>174.1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>516.39999999999986</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>391.69999999999891</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>250.99999999999901</v>
+      </c>
+      <c r="C12">
+        <v>283.39999999999998</v>
+      </c>
+      <c r="D12">
+        <v>137.5</v>
+      </c>
+      <c r="E12">
+        <v>283.39999999999998</v>
+      </c>
+      <c r="F12">
+        <v>261.69999999999902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>74.8</v>
+      </c>
+      <c r="C13">
+        <v>137</v>
+      </c>
+      <c r="D13">
+        <v>31.6999999999999</v>
+      </c>
+      <c r="E13">
+        <v>99.2</v>
+      </c>
+      <c r="F13">
+        <v>104.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10.6</v>
+      </c>
+      <c r="C14">
+        <v>84.2</v>
+      </c>
+      <c r="D14">
+        <v>16.5</v>
+      </c>
+      <c r="E14">
+        <v>60.5</v>
+      </c>
+      <c r="F14">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>58</v>
+      </c>
+      <c r="D15">
+        <v>3.5</v>
+      </c>
+      <c r="E15">
+        <v>39.599999999999902</v>
+      </c>
+      <c r="F15">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>26.299999999999901</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>18.7</v>
+      </c>
+      <c r="F16">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>12.8</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>SUM(A11:A17)</f>
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <f>SUM(B11:B18)</f>
+        <v>336.39999999999901</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C11:C18)</f>
+        <v>588.89999999999986</v>
+      </c>
+      <c r="D19">
+        <f>SUM(D11:D18)</f>
+        <v>189.1999999999999</v>
+      </c>
+      <c r="E19">
+        <f>SUM(E11:E18)</f>
+        <v>516.39999999999986</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19" si="1">SUM(F11:F17)</f>
+        <v>426.19999999999897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2 weeks of updates
</commit_message>
<xml_diff>
--- a/PowerGridResearch/Code/DCPF-MST/data.xlsx
+++ b/PowerGridResearch/Code/DCPF-MST/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian French\Documents\GitHub\PowerGridResearch\PowerGridResearch\Code\DCPF-MST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBC4B62-C83D-499A-AEEE-E57F01757641}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{500A55C8-4975-4B91-8B0C-3BBF194FF666}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34875" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="10890" firstSheet="2" activeTab="7" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus 30" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,11 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
     <sheet name="Resilience1" sheetId="6" r:id="rId5"/>
     <sheet name="Resilience12" sheetId="7" r:id="rId6"/>
+    <sheet name="MST vs Routing" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="182">
   <si>
     <t>timestep</t>
   </si>
@@ -117,6 +120,471 @@
   </si>
   <si>
     <t>Random Resilience</t>
+  </si>
+  <si>
+    <t>Routing on Geographic</t>
+  </si>
+  <si>
+    <t>Runtime: 639 sec to 3% gap</t>
+  </si>
+  <si>
+    <t>['L', 18, 0]</t>
+  </si>
+  <si>
+    <t>['L', 23, 0]</t>
+  </si>
+  <si>
+    <t>['L', 32, 1]</t>
+  </si>
+  <si>
+    <t>['L', 17, 2]</t>
+  </si>
+  <si>
+    <t>['L', 29, 2]</t>
+  </si>
+  <si>
+    <t>['L', 34, 2]</t>
+  </si>
+  <si>
+    <t>['L', 36, 2]</t>
+  </si>
+  <si>
+    <t>['L', 39, 2]</t>
+  </si>
+  <si>
+    <t>['N', 17, 3]</t>
+  </si>
+  <si>
+    <t>['N', 18, 3]</t>
+  </si>
+  <si>
+    <t>['N', 2, 4]</t>
+  </si>
+  <si>
+    <t>['N', 19, 4]</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>['N', 4, 0]</t>
+  </si>
+  <si>
+    <t>['N', 9, 1]</t>
+  </si>
+  <si>
+    <t>['L', 18, 1]</t>
+  </si>
+  <si>
+    <t>['L', 26, 1]</t>
+  </si>
+  <si>
+    <t>['N', 20, 2]</t>
+  </si>
+  <si>
+    <t>['L', 24, 2]</t>
+  </si>
+  <si>
+    <t>['L', 32, 2]</t>
+  </si>
+  <si>
+    <t>['N', 14, 3]</t>
+  </si>
+  <si>
+    <t>['N', 29, 3]</t>
+  </si>
+  <si>
+    <t>['N', 21, 4]</t>
+  </si>
+  <si>
+    <t>['L', 2, 4]</t>
+  </si>
+  <si>
+    <t>Random Scenario</t>
+  </si>
+  <si>
+    <t>Routing</t>
+  </si>
+  <si>
+    <t>MST</t>
+  </si>
+  <si>
+    <t>15s to 3% gap</t>
+  </si>
+  <si>
+    <t>488s to 3% gap</t>
+  </si>
+  <si>
+    <t>['L', 3, 0]</t>
+  </si>
+  <si>
+    <t>['N', 15, 1]</t>
+  </si>
+  <si>
+    <t>['L', 17, 1]</t>
+  </si>
+  <si>
+    <t>['L', 24, 1]</t>
+  </si>
+  <si>
+    <t>['N', 7, 2]</t>
+  </si>
+  <si>
+    <t>['N', 23, 3]</t>
+  </si>
+  <si>
+    <t>['N', 24, 4]</t>
+  </si>
+  <si>
+    <t>['L', 20, 4]</t>
+  </si>
+  <si>
+    <t>['L', 35, 4]</t>
+  </si>
+  <si>
+    <t>['L', 24, 0]</t>
+  </si>
+  <si>
+    <t>['N', 7, 1]</t>
+  </si>
+  <si>
+    <t>['L', 8, 1]</t>
+  </si>
+  <si>
+    <t>['L', 35, 1]</t>
+  </si>
+  <si>
+    <t>['N', 23, 2]</t>
+  </si>
+  <si>
+    <t>['L', 30, 2]</t>
+  </si>
+  <si>
+    <t>['N', 15, 4]</t>
+  </si>
+  <si>
+    <t>['L', 30, 0]</t>
+  </si>
+  <si>
+    <t>['N', 18, 2]</t>
+  </si>
+  <si>
+    <t>['N', 24, 3]</t>
+  </si>
+  <si>
+    <t>['N', 14, 1]</t>
+  </si>
+  <si>
+    <t>['L', 29, 1]</t>
+  </si>
+  <si>
+    <t>['N', 9, 2]</t>
+  </si>
+  <si>
+    <t>['N', 21, 3]</t>
+  </si>
+  <si>
+    <t>['L', 26, 3]</t>
+  </si>
+  <si>
+    <t>['N', 29, 4]</t>
+  </si>
+  <si>
+    <t>['L', 25, 4]</t>
+  </si>
+  <si>
+    <t>25s to 3% gap</t>
+  </si>
+  <si>
+    <t>57 Bus Scenario</t>
+  </si>
+  <si>
+    <t>['N', 7, 0]</t>
+  </si>
+  <si>
+    <t>['L', 1, 0]</t>
+  </si>
+  <si>
+    <t>['L', 2, 0]</t>
+  </si>
+  <si>
+    <t>['L', 48, 0]</t>
+  </si>
+  <si>
+    <t>['L', 58, 0]</t>
+  </si>
+  <si>
+    <t>['L', 60, 0]</t>
+  </si>
+  <si>
+    <t>['N', 35, 1]</t>
+  </si>
+  <si>
+    <t>['L', 3, 1]</t>
+  </si>
+  <si>
+    <t>['L', 4, 1]</t>
+  </si>
+  <si>
+    <t>['L', 77, 1]</t>
+  </si>
+  <si>
+    <t>['N', 15, 2]</t>
+  </si>
+  <si>
+    <t>['L', 26, 2]</t>
+  </si>
+  <si>
+    <t>['L', 44, 2]</t>
+  </si>
+  <si>
+    <t>['L', 45, 2]</t>
+  </si>
+  <si>
+    <t>['L', 74, 2]</t>
+  </si>
+  <si>
+    <t>['N', 39, 3]</t>
+  </si>
+  <si>
+    <t>['N', 55, 3]</t>
+  </si>
+  <si>
+    <t>['L', 54, 3]</t>
+  </si>
+  <si>
+    <t>['N', 17, 4]</t>
+  </si>
+  <si>
+    <t>['L', 9, 4]</t>
+  </si>
+  <si>
+    <t>['N', 38, 5]</t>
+  </si>
+  <si>
+    <t>[35, 55, 1.0]</t>
+  </si>
+  <si>
+    <t>[39, 34, 1.0]</t>
+  </si>
+  <si>
+    <t>4328s to 3%</t>
+  </si>
+  <si>
+    <t>Scenario 1 (geographic)</t>
+  </si>
+  <si>
+    <t>['N', 9, 0]</t>
+  </si>
+  <si>
+    <t>['L', 23, 1]</t>
+  </si>
+  <si>
+    <t>['L', 2, 2]</t>
+  </si>
+  <si>
+    <t>['L', 8, 2]</t>
+  </si>
+  <si>
+    <t>['L', 30, 3]</t>
+  </si>
+  <si>
+    <t>Road First</t>
+  </si>
+  <si>
+    <t>No Road Damage</t>
+  </si>
+  <si>
+    <t>No Road Repair</t>
+  </si>
+  <si>
+    <t>['N', 29, 2]</t>
+  </si>
+  <si>
+    <t>['L', 32, 3]</t>
+  </si>
+  <si>
+    <t>['L', 8, 4]</t>
+  </si>
+  <si>
+    <t>['L', 2, 3]</t>
+  </si>
+  <si>
+    <t>['L', 8, 3]</t>
+  </si>
+  <si>
+    <t>['L', 18, 3]</t>
+  </si>
+  <si>
+    <t>Scenario 2(Random)</t>
+  </si>
+  <si>
+    <t>Scenario 3(IISE)</t>
+  </si>
+  <si>
+    <t>['L', 17, 0]</t>
+  </si>
+  <si>
+    <t>['N', 23, 1]</t>
+  </si>
+  <si>
+    <t>['N', 24, 1]</t>
+  </si>
+  <si>
+    <t>['L', 20, 2]</t>
+  </si>
+  <si>
+    <t>['N', 15, 3]</t>
+  </si>
+  <si>
+    <t>['L', 14, 3]</t>
+  </si>
+  <si>
+    <t>no travel time</t>
+  </si>
+  <si>
+    <t>no travel</t>
+  </si>
+  <si>
+    <t>no roads</t>
+  </si>
+  <si>
+    <t>Damaged Roads</t>
+  </si>
+  <si>
+    <t>no road repair</t>
+  </si>
+  <si>
+    <t>Scenario4 (57 bus)</t>
+  </si>
+  <si>
+    <t>no road damage</t>
+  </si>
+  <si>
+    <t>damaged roads</t>
+  </si>
+  <si>
+    <t>['N', 14, 0]</t>
+  </si>
+  <si>
+    <t>['N', 20, 1]</t>
+  </si>
+  <si>
+    <t>['N', 21, 2]</t>
+  </si>
+  <si>
+    <t>['L', 25, 3]</t>
+  </si>
+  <si>
+    <t>N,4,0</t>
+  </si>
+  <si>
+    <t>L,23,0</t>
+  </si>
+  <si>
+    <t>L,24,0</t>
+  </si>
+  <si>
+    <t>Post Processed</t>
+  </si>
+  <si>
+    <t>N,20,1</t>
+  </si>
+  <si>
+    <t>L,29,1</t>
+  </si>
+  <si>
+    <t>L,26,1</t>
+  </si>
+  <si>
+    <t>N,14,2</t>
+  </si>
+  <si>
+    <t>N,21,3</t>
+  </si>
+  <si>
+    <t>L,32,3</t>
+  </si>
+  <si>
+    <t>L,2,3</t>
+  </si>
+  <si>
+    <t>N,29,4</t>
+  </si>
+  <si>
+    <t>L,25,4</t>
+  </si>
+  <si>
+    <t>L,18,4</t>
+  </si>
+  <si>
+    <t>N,9,5</t>
+  </si>
+  <si>
+    <t>L,8,5</t>
+  </si>
+  <si>
+    <t>['L', 2, 1]</t>
+  </si>
+  <si>
+    <t>['L', 30, 1]</t>
+  </si>
+  <si>
+    <t>['L', 35, 3]</t>
+  </si>
+  <si>
+    <t>['N', 24, 2]</t>
+  </si>
+  <si>
+    <t>['L', 17, 3]</t>
+  </si>
+  <si>
+    <t>['L', 24, 3]</t>
+  </si>
+  <si>
+    <t>N-7-0</t>
+  </si>
+  <si>
+    <t>L-17-0</t>
+  </si>
+  <si>
+    <t>L-3-0</t>
+  </si>
+  <si>
+    <t>N-4-1</t>
+  </si>
+  <si>
+    <t>L-35-1</t>
+  </si>
+  <si>
+    <t>N-24-2</t>
+  </si>
+  <si>
+    <t>L-30-3</t>
+  </si>
+  <si>
+    <t>N-23-2</t>
+  </si>
+  <si>
+    <t>N-18-3</t>
+  </si>
+  <si>
+    <t>L-2-3</t>
+  </si>
+  <si>
+    <t>L-8-3</t>
+  </si>
+  <si>
+    <t>L-20-3</t>
+  </si>
+  <si>
+    <t>N-15-4</t>
+  </si>
+  <si>
+    <t>L-24-4</t>
+  </si>
+  <si>
+    <t>L-14-3</t>
   </si>
 </sst>
 </file>
@@ -152,8 +620,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6804,19 +7273,19 @@
         <v>181.5</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:F11" si="0">SUM(C2)</f>
+        <f>SUM(C2)</f>
         <v>181.5</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>SUM(D2)</f>
         <v>181.5</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>SUM(E2)</f>
         <v>181.5</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f>SUM(F2)</f>
         <v>181.5</v>
       </c>
     </row>
@@ -6829,19 +7298,19 @@
         <v>256</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:F12" si="1">SUM(C2:C3)</f>
+        <f>SUM(C2:C3)</f>
         <v>324.7</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f>SUM(D2:D3)</f>
         <v>363</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f>SUM(E2:E3)</f>
         <v>256.3</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f>SUM(F2:F3)</f>
         <v>256.3</v>
       </c>
     </row>
@@ -6854,19 +7323,19 @@
         <v>305</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:F13" si="2">SUM(C2:C4)</f>
+        <f>SUM(C2:C4)</f>
         <v>450.4</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
+        <f>SUM(D2:D4)</f>
         <v>437.8</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f>SUM(E2:E4)</f>
         <v>296.10000000000002</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f>SUM(F2:F4)</f>
         <v>331.1</v>
       </c>
     </row>
@@ -6879,19 +7348,19 @@
         <v>336.5</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:F14" si="3">SUM(C2:C5)</f>
+        <f>SUM(C2:C5)</f>
         <v>576.1</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
+        <f>SUM(D2:D5)</f>
         <v>486.8</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
+        <f>SUM(E2:E5)</f>
         <v>324.20000000000005</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f>SUM(F2:F5)</f>
         <v>370.90000000000003</v>
       </c>
     </row>
@@ -6904,19 +7373,19 @@
         <v>347.1</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:F15" si="4">SUM(C2:C6)</f>
+        <f>SUM(C2:C6)</f>
         <v>680.9</v>
       </c>
       <c r="D15">
-        <f t="shared" si="4"/>
+        <f>SUM(D2:D6)</f>
         <v>518.29999999999995</v>
       </c>
       <c r="E15">
-        <f t="shared" si="4"/>
+        <f>SUM(E2:E6)</f>
         <v>334.80000000000007</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
+        <f>SUM(F2:F6)</f>
         <v>399.00000000000006</v>
       </c>
     </row>
@@ -6929,19 +7398,19 @@
         <v>357.70000000000005</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:F16" si="5">SUM(C2:C7)</f>
+        <f>SUM(C2:C7)</f>
         <v>785.69999999999993</v>
       </c>
       <c r="D16">
-        <f t="shared" si="5"/>
+        <f>SUM(D2:D7)</f>
         <v>528.9</v>
       </c>
       <c r="E16">
-        <f t="shared" si="5"/>
+        <f>SUM(E2:E7)</f>
         <v>345.40000000000009</v>
       </c>
       <c r="F16">
-        <f t="shared" si="5"/>
+        <f>SUM(F2:F7)</f>
         <v>409.60000000000008</v>
       </c>
     </row>
@@ -7196,19 +7665,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f t="shared" ref="B11:E11" si="0">SUM(B2:B7)</f>
+        <f>SUM(B2:B7)</f>
         <v>1002.1</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>SUM(C2:C7)</f>
         <v>966.69999999999777</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>SUM(D2:D7)</f>
         <v>907.09999999999877</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>SUM(E2:E7)</f>
         <v>1008.3999999999999</v>
       </c>
       <c r="F11">
@@ -7387,7 +7856,7 @@
         <v>559.39999999999884</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:F8" si="0">SUM(C2:C7)</f>
+        <f>SUM(C2:C7)</f>
         <v>634.599999999999</v>
       </c>
       <c r="D8">
@@ -7395,11 +7864,11 @@
         <v>676.39999999999873</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>SUM(E2:E7)</f>
         <v>443.99999999999881</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>SUM(F2:F7)</f>
         <v>635.1</v>
       </c>
     </row>
@@ -7889,7 +8358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946CCB79-A94E-4848-8DCC-31F38FA0F6DB}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -8238,8 +8707,1985 @@
         <v>516.39999999999986</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19" si="1">SUM(F11:F17)</f>
+        <f>SUM(F11:F17)</f>
         <v>426.19999999999897</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DA80CB-66C0-401E-9850-C46E94BA8684}">
+  <dimension ref="A4:K58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>187.69999999999899</v>
+      </c>
+      <c r="B5">
+        <v>187.69999999999899</v>
+      </c>
+      <c r="F5">
+        <v>219.7</v>
+      </c>
+      <c r="G5">
+        <v>219.7</v>
+      </c>
+      <c r="K5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>87.3</v>
+      </c>
+      <c r="B6">
+        <v>74.8</v>
+      </c>
+      <c r="F6">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="G6">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="K6">
+        <v>777.79999999999905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>52.5</v>
+      </c>
+      <c r="B7">
+        <v>48.8</v>
+      </c>
+      <c r="F7">
+        <v>64.7</v>
+      </c>
+      <c r="G7">
+        <v>40.4</v>
+      </c>
+      <c r="K7">
+        <v>627.79999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>31.5</v>
+      </c>
+      <c r="B8">
+        <v>23.299999999999901</v>
+      </c>
+      <c r="F8">
+        <v>34.699999999999903</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="K8">
+        <v>389.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10.6</v>
+      </c>
+      <c r="B9">
+        <v>10.6</v>
+      </c>
+      <c r="F9">
+        <v>16.5</v>
+      </c>
+      <c r="G9">
+        <v>3.5</v>
+      </c>
+      <c r="K9">
+        <v>328.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>3.5</v>
+      </c>
+      <c r="K10">
+        <v>314.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>SUM(A5:A10)</f>
+        <v>369.599999999999</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B5:B10)</f>
+        <v>345.19999999999891</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F5:F10)</f>
+        <v>405.99999999999989</v>
+      </c>
+      <c r="G11">
+        <f>SUM(G5:G10)</f>
+        <v>357.5</v>
+      </c>
+      <c r="K11">
+        <v>309.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12">
+        <f>SUM(K6:K11)</f>
+        <v>2747.9999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" t="s">
+        <v>75</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
+        <v>76</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" t="s">
+        <v>73</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="K42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="K44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="K46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="K48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="K50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="K52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="K54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="K56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>40</v>
+      </c>
+      <c r="K57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F860931-E7EC-4A58-BCA4-59BD69D58A1B}">
+  <dimension ref="A11:X57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" t="s">
+        <v>125</v>
+      </c>
+      <c r="P11" t="s">
+        <v>126</v>
+      </c>
+      <c r="V11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" t="s">
+        <v>137</v>
+      </c>
+      <c r="L12" t="s">
+        <v>148</v>
+      </c>
+      <c r="P12" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R12" t="s">
+        <v>133</v>
+      </c>
+      <c r="S12" t="s">
+        <v>136</v>
+      </c>
+      <c r="V12" t="s">
+        <v>116</v>
+      </c>
+      <c r="W12" t="s">
+        <v>139</v>
+      </c>
+      <c r="X12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>187.69999999999899</v>
+      </c>
+      <c r="C13">
+        <v>187.69999999999899</v>
+      </c>
+      <c r="D13">
+        <v>187.69999999999899</v>
+      </c>
+      <c r="E13">
+        <v>187.7</v>
+      </c>
+      <c r="H13">
+        <v>219.69999999999399</v>
+      </c>
+      <c r="J13">
+        <v>219.7</v>
+      </c>
+      <c r="K13">
+        <v>219.69999999999399</v>
+      </c>
+      <c r="L13">
+        <v>219.7</v>
+      </c>
+      <c r="P13">
+        <v>181.70000000000101</v>
+      </c>
+      <c r="R13">
+        <v>181.69999999998899</v>
+      </c>
+      <c r="S13">
+        <v>181.69999999998899</v>
+      </c>
+      <c r="V13">
+        <v>647.99999999999898</v>
+      </c>
+      <c r="W13">
+        <v>647.99999999999898</v>
+      </c>
+      <c r="X13">
+        <v>647.99999999999898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>69.899999999999906</v>
+      </c>
+      <c r="B14">
+        <v>187.69999999999899</v>
+      </c>
+      <c r="C14">
+        <v>69.899999999999906</v>
+      </c>
+      <c r="D14">
+        <v>48.8</v>
+      </c>
+      <c r="E14">
+        <v>74.8</v>
+      </c>
+      <c r="H14">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="I14">
+        <v>219.69999999999399</v>
+      </c>
+      <c r="J14">
+        <v>38.199999999999903</v>
+      </c>
+      <c r="K14">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="L14">
+        <v>132.4</v>
+      </c>
+      <c r="P14">
+        <v>98.700000004751899</v>
+      </c>
+      <c r="Q14">
+        <v>181.69999999998899</v>
+      </c>
+      <c r="R14">
+        <v>60.5</v>
+      </c>
+      <c r="S14">
+        <v>98.7</v>
+      </c>
+      <c r="V14">
+        <v>140.09999999984501</v>
+      </c>
+      <c r="W14">
+        <v>140.1</v>
+      </c>
+      <c r="X14">
+        <v>140.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>28.1</v>
+      </c>
+      <c r="B15">
+        <v>69.899999999999906</v>
+      </c>
+      <c r="C15">
+        <v>28.1</v>
+      </c>
+      <c r="D15">
+        <v>10.6</v>
+      </c>
+      <c r="E15">
+        <v>36.4</v>
+      </c>
+      <c r="H15">
+        <v>40.4</v>
+      </c>
+      <c r="I15">
+        <v>68.2</v>
+      </c>
+      <c r="J15">
+        <v>13</v>
+      </c>
+      <c r="K15">
+        <v>40.4</v>
+      </c>
+      <c r="L15">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="P15">
+        <v>66.700000006996902</v>
+      </c>
+      <c r="Q15">
+        <v>83.8</v>
+      </c>
+      <c r="R15">
+        <v>40.099999999999902</v>
+      </c>
+      <c r="S15">
+        <v>66.699998449999995</v>
+      </c>
+      <c r="V15">
+        <v>72.349999999999895</v>
+      </c>
+      <c r="W15">
+        <v>72.349999999999994</v>
+      </c>
+      <c r="X15">
+        <v>72.349999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5.9999999999999902</v>
+      </c>
+      <c r="B16">
+        <v>28.1</v>
+      </c>
+      <c r="C16">
+        <v>5.9999999999999902</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>36.4</v>
+      </c>
+      <c r="H16">
+        <v>15.2</v>
+      </c>
+      <c r="I16">
+        <v>29.5</v>
+      </c>
+      <c r="J16">
+        <v>3.5</v>
+      </c>
+      <c r="K16">
+        <v>25.2</v>
+      </c>
+      <c r="L16">
+        <v>13</v>
+      </c>
+      <c r="P16">
+        <v>51.500000008780901</v>
+      </c>
+      <c r="Q16">
+        <v>51.5</v>
+      </c>
+      <c r="R16">
+        <v>28.1999999999999</v>
+      </c>
+      <c r="S16">
+        <v>51.5</v>
+      </c>
+      <c r="V16">
+        <v>45.099999999999902</v>
+      </c>
+      <c r="W16">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="X16">
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>32.5</v>
+      </c>
+      <c r="H17">
+        <v>3.4999999999999898</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>16.5</v>
+      </c>
+      <c r="L17">
+        <v>3.5</v>
+      </c>
+      <c r="P17">
+        <v>30.600000011239</v>
+      </c>
+      <c r="Q17">
+        <v>30.6</v>
+      </c>
+      <c r="R17">
+        <v>15.2</v>
+      </c>
+      <c r="S17">
+        <v>36.899999724637603</v>
+      </c>
+      <c r="V17">
+        <v>25.799999999999901</v>
+      </c>
+      <c r="W17">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="X17">
+        <v>25.799999999999901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>18.700000013065999</v>
+      </c>
+      <c r="Q18">
+        <v>18.6999992068125</v>
+      </c>
+      <c r="R18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S18">
+        <v>18.7</v>
+      </c>
+      <c r="V18">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="W18">
+        <v>5</v>
+      </c>
+      <c r="X18">
+        <v>16.400000105479901</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>SUM(A13:A18)</f>
+        <v>291.69999999999891</v>
+      </c>
+      <c r="B19">
+        <f>SUM(B13:B18)</f>
+        <v>291.69999999999891</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>15.2</v>
+      </c>
+      <c r="V19">
+        <v>5</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>4.9999957123654504</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" t="s">
+        <v>146</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" t="s">
+        <v>86</v>
+      </c>
+      <c r="K29" t="s">
+        <v>58</v>
+      </c>
+      <c r="L29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" t="s">
+        <v>58</v>
+      </c>
+      <c r="K31" t="s">
+        <v>68</v>
+      </c>
+      <c r="L31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
+        <v>149</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" t="s">
+        <v>127</v>
+      </c>
+      <c r="K33" t="s">
+        <v>161</v>
+      </c>
+      <c r="L33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>150</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" t="s">
+        <v>128</v>
+      </c>
+      <c r="K35" t="s">
+        <v>61</v>
+      </c>
+      <c r="L35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" t="s">
+        <v>151</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>70</v>
+      </c>
+      <c r="J37" t="s">
+        <v>129</v>
+      </c>
+      <c r="K37" t="s">
+        <v>162</v>
+      </c>
+      <c r="L37" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>71</v>
+      </c>
+      <c r="J39" t="s">
+        <v>70</v>
+      </c>
+      <c r="K39" t="s">
+        <v>96</v>
+      </c>
+      <c r="L39" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" t="s">
+        <v>153</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>164</v>
+      </c>
+      <c r="J41" t="s">
+        <v>75</v>
+      </c>
+      <c r="K41" t="s">
+        <v>75</v>
+      </c>
+      <c r="L41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>72</v>
+      </c>
+      <c r="J43" t="s">
+        <v>113</v>
+      </c>
+      <c r="K43" t="s">
+        <v>32</v>
+      </c>
+      <c r="L43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" t="s">
+        <v>155</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>38</v>
+      </c>
+      <c r="J45" t="s">
+        <v>114</v>
+      </c>
+      <c r="K45" t="s">
+        <v>63</v>
+      </c>
+      <c r="L45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" t="s">
+        <v>156</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>132</v>
+      </c>
+      <c r="J47" t="s">
+        <v>130</v>
+      </c>
+      <c r="K47" t="s">
+        <v>123</v>
+      </c>
+      <c r="L47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48" t="s">
+        <v>157</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>0.999999999999999</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>165</v>
+      </c>
+      <c r="J49" t="s">
+        <v>47</v>
+      </c>
+      <c r="K49" t="s">
+        <v>132</v>
+      </c>
+      <c r="L49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" t="s">
+        <v>158</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>166</v>
+      </c>
+      <c r="J51" t="s">
+        <v>72</v>
+      </c>
+      <c r="K51" t="s">
+        <v>163</v>
+      </c>
+      <c r="L51" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>73</v>
+      </c>
+      <c r="J53" t="s">
+        <v>131</v>
+      </c>
+      <c r="K53" t="s">
+        <v>64</v>
+      </c>
+      <c r="L53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" t="s">
+        <v>160</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>0.999999999999999</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>65</v>
+      </c>
+      <c r="J55" t="s">
+        <v>132</v>
+      </c>
+      <c r="L55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>83</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more data and 3 pages of thesis
</commit_message>
<xml_diff>
--- a/PowerGridResearch/Code/DCPF-MST/data.xlsx
+++ b/PowerGridResearch/Code/DCPF-MST/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian French\Documents\GitHub\PowerGridResearch\PowerGridResearch\Code\DCPF-MST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2B118-02B9-4244-B1C1-004EEE70AB40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D02809-DE8C-4D5D-82E4-562D590D1895}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-165" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
+    <workbookView xWindow="57480" yWindow="-165" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{F89CF7D2-7D69-49DF-9B99-C93E6F5D4608}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus 30" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Resilience12" sheetId="7" r:id="rId6"/>
     <sheet name="MST vs Routing" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="223">
   <si>
     <t>timestep</t>
   </si>
@@ -118,9 +119,6 @@
     <t>Optimal Resilience</t>
   </si>
   <si>
-    <t>Random Resilience</t>
-  </si>
-  <si>
     <t>Routing on Geographic</t>
   </si>
   <si>
@@ -638,6 +636,78 @@
   </si>
   <si>
     <t>[[[9, 1, 'node']], [[23, 2, 'edge']], [[26, 2, 'edge']]]</t>
+  </si>
+  <si>
+    <t>No Travel Time</t>
+  </si>
+  <si>
+    <t>['N', 11, 0]</t>
+  </si>
+  <si>
+    <t>['L', 31, 0]</t>
+  </si>
+  <si>
+    <t>['L', 40, 0]</t>
+  </si>
+  <si>
+    <t>['N', 4, 1]</t>
+  </si>
+  <si>
+    <t>['N', 28, 1]</t>
+  </si>
+  <si>
+    <t>['L', 7, 1]</t>
+  </si>
+  <si>
+    <t>['L', 12, 1]</t>
+  </si>
+  <si>
+    <t>['L', 41, 2]</t>
+  </si>
+  <si>
+    <t>['L', 42, 2]</t>
+  </si>
+  <si>
+    <t>['N', 31, 3]</t>
+  </si>
+  <si>
+    <t>['L', 44, 3]</t>
+  </si>
+  <si>
+    <t>['L', 52, 3]</t>
+  </si>
+  <si>
+    <t>['N', 9, 4]</t>
+  </si>
+  <si>
+    <t>['L', 18, 4]</t>
+  </si>
+  <si>
+    <t>['L', 63, 5]</t>
+  </si>
+  <si>
+    <t>[[[14, 0, 'node']], [[40, 0, 'edge']], [[31, 0, 'edge']]]</t>
+  </si>
+  <si>
+    <t>[[[11, 0, 'node']], [[12, 1, 'edge']], [[7, 1, 'edge']]]</t>
+  </si>
+  <si>
+    <t>[[[28, 1, 'node']], [[21, 2, 'node']]]</t>
+  </si>
+  <si>
+    <t>[[[20, 2, 'node']], [[42, 2, 'edge']], [[41, 2, 'edge']], [[44, 3, 'edge']], [[52, 3, 'edge']]]</t>
+  </si>
+  <si>
+    <t>[[[31, 3, 'node']], [[20, 4, 'edge']], [[18, 4, 'edge']]]</t>
+  </si>
+  <si>
+    <t>[[[29, 3, 'node']], [[63, 5, 'edge']]]</t>
+  </si>
+  <si>
+    <t>Heuristic Resilience</t>
+  </si>
+  <si>
+    <t>No Resilience</t>
   </si>
 </sst>
 </file>
@@ -8409,10 +8479,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946CCB79-A94E-4848-8DCC-31F38FA0F6DB}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8427,87 +8497,72 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>250.99999999999901</v>
+        <v>123.4</v>
       </c>
       <c r="C2">
-        <v>283.39999999999998</v>
+        <v>221.7</v>
       </c>
       <c r="D2">
-        <v>107.1</v>
+        <v>174.1</v>
       </c>
       <c r="E2">
-        <v>283.39999999999998</v>
-      </c>
-      <c r="F2">
-        <v>259.29999999999899</v>
+        <v>179.3</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>55.8</v>
+        <v>67.2</v>
       </c>
       <c r="C3">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D3">
-        <v>37.6</v>
+        <v>104.7</v>
       </c>
       <c r="E3">
-        <v>99.2</v>
-      </c>
-      <c r="F3">
-        <v>73.599999999999994</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>14.1</v>
+        <v>43.7</v>
       </c>
       <c r="C4">
-        <v>84.2</v>
+        <v>51.7</v>
       </c>
       <c r="D4">
-        <v>22.4</v>
+        <v>60.7</v>
       </c>
       <c r="E4">
-        <v>60.5</v>
-      </c>
-      <c r="F4">
-        <v>40.4</v>
+        <v>41.4</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>0</v>
+        <v>16.7</v>
       </c>
       <c r="C5">
-        <v>58</v>
+        <v>16.2</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>22.2</v>
       </c>
       <c r="E5">
-        <v>39.599999999999902</v>
-      </c>
-      <c r="F5">
-        <v>14.9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6">
+        <v>2.4</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>26.299999999999901</v>
-      </c>
       <c r="D6">
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="E6">
-        <v>18.7</v>
-      </c>
-      <c r="F6">
-        <v>3.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -8518,12 +8573,9 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5.9</v>
       </c>
       <c r="E7">
-        <v>12.8</v>
-      </c>
-      <c r="F7">
         <v>0</v>
       </c>
     </row>
@@ -8538,9 +8590,6 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F8">
         <v>0</v>
       </c>
     </row>
@@ -8551,23 +8600,23 @@
       </c>
       <c r="B9">
         <f t="shared" ref="B9:Q9" si="0">SUM(B2:B8)</f>
-        <v>320.89999999999901</v>
+        <v>253.4</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>588.89999999999986</v>
+        <v>437.59999999999997</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>174.1</v>
+        <v>375.7</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>516.39999999999986</v>
+        <v>322.60000000000002</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>391.69999999999891</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -8616,92 +8665,77 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>250.99999999999901</v>
+        <v>123.4</v>
       </c>
       <c r="C12">
-        <v>283.39999999999998</v>
+        <v>181.7</v>
       </c>
       <c r="D12">
-        <v>137.5</v>
+        <v>174.1</v>
       </c>
       <c r="E12">
-        <v>283.39999999999998</v>
-      </c>
-      <c r="F12">
-        <v>261.69999999999902</v>
+        <v>179.3</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>74.8</v>
+        <v>93.5</v>
       </c>
       <c r="C13">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="D13">
-        <v>31.6999999999999</v>
+        <v>104.7</v>
       </c>
       <c r="E13">
-        <v>99.2</v>
-      </c>
-      <c r="F13">
-        <v>104.7</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>10.6</v>
+        <v>43.7</v>
       </c>
       <c r="C14">
-        <v>84.2</v>
+        <v>51.7</v>
       </c>
       <c r="D14">
-        <v>16.5</v>
+        <v>54.5</v>
       </c>
       <c r="E14">
-        <v>60.5</v>
-      </c>
-      <c r="F14">
         <v>41.4</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>0</v>
+        <v>16.7</v>
       </c>
       <c r="C15">
-        <v>58</v>
+        <v>16.2</v>
       </c>
       <c r="D15">
-        <v>3.5</v>
+        <v>42</v>
       </c>
       <c r="E15">
-        <v>39.599999999999902</v>
-      </c>
-      <c r="F15">
-        <v>14.9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
         <v>0</v>
       </c>
-      <c r="C16">
-        <v>26.299999999999901</v>
-      </c>
       <c r="D16">
-        <v>0</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E16">
-        <v>18.7</v>
-      </c>
-      <c r="F16">
-        <v>3.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -8715,9 +8749,6 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>12.8</v>
-      </c>
-      <c r="F17">
         <v>0</v>
       </c>
     </row>
@@ -8732,9 +8763,6 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F18">
         <v>0</v>
       </c>
     </row>
@@ -8745,27 +8773,157 @@
       </c>
       <c r="B19">
         <f>SUM(B11:B18)</f>
-        <v>336.39999999999901</v>
+        <v>283.3</v>
       </c>
       <c r="C19">
         <f>SUM(C11:C18)</f>
-        <v>588.89999999999986</v>
+        <v>330.59999999999997</v>
       </c>
       <c r="D19">
         <f>SUM(D11:D18)</f>
-        <v>189.1999999999999</v>
+        <v>379.90000000000003</v>
       </c>
       <c r="E19">
         <f>SUM(E11:E18)</f>
-        <v>516.39999999999986</v>
+        <v>322.60000000000002</v>
       </c>
       <c r="F19">
         <f>SUM(F11:F17)</f>
-        <v>426.19999999999897</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>123.4</v>
+      </c>
+      <c r="C22">
+        <v>231.7</v>
+      </c>
+      <c r="D22">
+        <v>174.1</v>
+      </c>
+      <c r="E22">
+        <v>179.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>82.1</v>
+      </c>
+      <c r="C23">
+        <v>127.5</v>
+      </c>
+      <c r="D23">
+        <v>104.7</v>
+      </c>
+      <c r="E23">
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>58.5</v>
+      </c>
+      <c r="C24">
+        <v>74.8</v>
+      </c>
+      <c r="D24">
+        <v>63.2</v>
+      </c>
+      <c r="E24">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>26.2</v>
+      </c>
+      <c r="C25">
+        <v>40.6</v>
+      </c>
+      <c r="D25">
+        <v>42</v>
+      </c>
+      <c r="E25">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>9.5</v>
+      </c>
+      <c r="C26">
+        <v>16.2</v>
+      </c>
+      <c r="D26">
+        <v>18.7</v>
+      </c>
+      <c r="E26">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2.4</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E27">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>SUM(A21:A27)</f>
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <f>SUM(B21:B28)</f>
+        <v>302.09999999999997</v>
+      </c>
+      <c r="C29">
+        <f>SUM(C21:C28)</f>
+        <v>490.8</v>
+      </c>
+      <c r="D29">
+        <f>SUM(D21:D28)</f>
+        <v>404.9</v>
+      </c>
+      <c r="E29">
+        <f>SUM(E21:E28)</f>
+        <v>338</v>
+      </c>
+      <c r="F29">
+        <f>SUM(F21:F27)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8786,19 +8944,19 @@
   <sheetData>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>54</v>
       </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -8815,7 +8973,7 @@
         <v>219.7</v>
       </c>
       <c r="K5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -8926,16 +9084,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K12">
         <f>SUM(K6:K11)</f>
@@ -8944,29 +9102,29 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -8986,21 +9144,21 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -9020,21 +9178,21 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -9054,21 +9212,21 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" t="s">
         <v>67</v>
-      </c>
-      <c r="F21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" t="s">
-        <v>68</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -9088,21 +9246,21 @@
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -9122,21 +9280,21 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -9156,21 +9314,21 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -9190,21 +9348,21 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -9224,21 +9382,21 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -9258,21 +9416,21 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -9292,21 +9450,21 @@
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -9326,15 +9484,15 @@
         <v>1</v>
       </c>
       <c r="K36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K37">
         <v>1</v>
@@ -9348,15 +9506,15 @@
         <v>1</v>
       </c>
       <c r="K38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -9370,12 +9528,12 @@
         <v>1</v>
       </c>
       <c r="K40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K41">
         <v>1</v>
@@ -9386,12 +9544,12 @@
         <v>1</v>
       </c>
       <c r="K42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K43">
         <v>1</v>
@@ -9402,12 +9560,12 @@
         <v>1</v>
       </c>
       <c r="K44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -9418,12 +9576,12 @@
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -9434,12 +9592,12 @@
         <v>1</v>
       </c>
       <c r="K48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K49">
         <v>1</v>
@@ -9450,12 +9608,12 @@
         <v>1</v>
       </c>
       <c r="K50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -9466,12 +9624,12 @@
         <v>1</v>
       </c>
       <c r="K52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K53">
         <v>1</v>
@@ -9482,12 +9640,12 @@
         <v>1</v>
       </c>
       <c r="K54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -9498,15 +9656,15 @@
         <v>1</v>
       </c>
       <c r="K56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
@@ -9521,10 +9679,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F860931-E7EC-4A58-BCA4-59BD69D58A1B}">
-  <dimension ref="A11:AG69"/>
+  <dimension ref="A11:AJ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
+    <sheetView topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9539,97 +9697,108 @@
     <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" customWidth="1"/>
+    <col min="31" max="31" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="P11" t="s">
         <v>125</v>
       </c>
-      <c r="P11" t="s">
-        <v>126</v>
-      </c>
       <c r="V11" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" t="s">
+        <v>136</v>
+      </c>
+      <c r="L12" t="s">
+        <v>147</v>
+      </c>
+      <c r="P12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>134</v>
+      </c>
+      <c r="R12" t="s">
+        <v>132</v>
+      </c>
+      <c r="S12" t="s">
+        <v>135</v>
+      </c>
+      <c r="V12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W12" t="s">
         <v>138</v>
       </c>
-      <c r="AA11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" t="s">
-        <v>148</v>
-      </c>
-      <c r="H12" t="s">
-        <v>116</v>
-      </c>
-      <c r="I12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12" t="s">
-        <v>134</v>
-      </c>
-      <c r="K12" t="s">
-        <v>137</v>
-      </c>
-      <c r="L12" t="s">
-        <v>148</v>
-      </c>
-      <c r="P12" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="X12" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE12" t="s">
         <v>135</v>
       </c>
-      <c r="R12" t="s">
-        <v>133</v>
-      </c>
-      <c r="S12" t="s">
-        <v>136</v>
-      </c>
-      <c r="V12" t="s">
-        <v>116</v>
-      </c>
-      <c r="W12" t="s">
-        <v>139</v>
-      </c>
-      <c r="X12" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>116</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC12" t="s">
+      <c r="AF12" t="s">
         <v>2</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AG12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH12" t="s">
         <v>184</v>
       </c>
-      <c r="AE12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>187.69999999999899</v>
       </c>
@@ -9672,26 +9841,35 @@
       <c r="X13">
         <v>647.99999999999898</v>
       </c>
-      <c r="AA13">
-        <v>240.49999999999901</v>
-      </c>
-      <c r="AB13">
-        <v>240.49999999999901</v>
-      </c>
-      <c r="AC13">
-        <v>240.5</v>
+      <c r="Y13">
+        <v>648</v>
+      </c>
+      <c r="Z13">
+        <v>648</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>215</v>
       </c>
       <c r="AD13">
         <v>240.49999999999901</v>
       </c>
       <c r="AE13">
+        <v>240.49999999999901</v>
+      </c>
+      <c r="AF13">
         <v>240.5</v>
       </c>
-      <c r="AG13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG13">
+        <v>240.49999999999901</v>
+      </c>
+      <c r="AH13">
+        <v>240.5</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>69.899999999999906</v>
       </c>
@@ -9743,26 +9921,35 @@
       <c r="X14">
         <v>140.1</v>
       </c>
-      <c r="AA14">
+      <c r="Y14">
+        <v>118.1</v>
+      </c>
+      <c r="Z14">
+        <v>543</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD14">
         <v>211.49999999999901</v>
       </c>
-      <c r="AB14">
+      <c r="AE14">
         <v>211.49999999999901</v>
       </c>
-      <c r="AC14">
+      <c r="AF14">
         <v>240.49999999999901</v>
       </c>
-      <c r="AD14">
+      <c r="AG14">
         <v>93.5</v>
       </c>
-      <c r="AE14">
+      <c r="AH14">
         <v>123.5</v>
       </c>
-      <c r="AG14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>28.1</v>
       </c>
@@ -9814,26 +10001,35 @@
       <c r="X15">
         <v>72.349999999999994</v>
       </c>
-      <c r="AA15">
+      <c r="Y15">
+        <v>52.3</v>
+      </c>
+      <c r="Z15">
+        <v>118.1</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>217</v>
+      </c>
+      <c r="AD15">
         <v>117.3</v>
       </c>
-      <c r="AB15">
+      <c r="AE15">
         <v>117.3</v>
       </c>
-      <c r="AC15">
+      <c r="AF15">
         <v>117.3</v>
       </c>
-      <c r="AD15">
+      <c r="AG15">
         <v>55.8</v>
       </c>
-      <c r="AE15">
+      <c r="AH15">
         <v>93.5</v>
       </c>
-      <c r="AG15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5.9999999999999902</v>
       </c>
@@ -9885,26 +10081,35 @@
       <c r="X16">
         <v>45.1</v>
       </c>
-      <c r="AA16">
+      <c r="Y16">
+        <v>25.799999999999901</v>
+      </c>
+      <c r="Z16">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD16">
         <v>87.3</v>
       </c>
-      <c r="AB16">
+      <c r="AE16">
         <v>87.300000000002896</v>
       </c>
-      <c r="AC16">
+      <c r="AF16">
         <v>72.5</v>
       </c>
-      <c r="AD16">
+      <c r="AG16">
         <v>29.5</v>
       </c>
-      <c r="AE16">
+      <c r="AH16">
         <v>67.099999999999994</v>
       </c>
-      <c r="AG16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -9956,26 +10161,35 @@
       <c r="X17">
         <v>25.799999999999901</v>
       </c>
-      <c r="AA17">
+      <c r="Y17">
+        <v>5</v>
+      </c>
+      <c r="Z17">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD17">
         <v>69.299994199999901</v>
       </c>
-      <c r="AB17">
+      <c r="AE17">
         <v>72.5</v>
       </c>
-      <c r="AC17">
+      <c r="AF17">
         <v>40.399999457019597</v>
       </c>
-      <c r="AD17">
+      <c r="AG17">
         <v>14.399999999999901</v>
       </c>
-      <c r="AE17">
+      <c r="AH17">
         <v>55.7</v>
       </c>
-      <c r="AG17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -10027,23 +10241,32 @@
       <c r="X18">
         <v>16.400000105479901</v>
       </c>
-      <c r="AA18">
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD18">
         <v>46.099994199999998</v>
       </c>
-      <c r="AB18">
+      <c r="AE18">
         <v>55</v>
       </c>
-      <c r="AC18">
+      <c r="AF18">
         <v>28.6999999999999</v>
       </c>
-      <c r="AD18">
+      <c r="AG18">
         <v>3.4999999999999898</v>
       </c>
-      <c r="AE18">
+      <c r="AH18">
         <v>55.7</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>SUM(A13:A18)</f>
         <v>291.69999999999891</v>
@@ -10067,11 +10290,17 @@
       <c r="X19">
         <v>4.9999957123654504</v>
       </c>
-      <c r="AC19">
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>18</v>
+      </c>
+      <c r="AF19">
         <v>14.1</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="V20">
         <v>0</v>
       </c>
@@ -10081,781 +10310,868 @@
       <c r="X20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA21" t="s">
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AD21" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG21" t="s">
         <v>183</v>
       </c>
-      <c r="AC21" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>184</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA22">
-        <v>240.49999999999901</v>
-      </c>
-      <c r="AB22">
-        <v>240.49999999999901</v>
-      </c>
-      <c r="AC22">
-        <v>240.49999999999901</v>
+      <c r="AH21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y22" t="s">
+        <v>200</v>
       </c>
       <c r="AD22">
         <v>240.49999999999901</v>
       </c>
       <c r="AE22">
+        <v>240.49999999999901</v>
+      </c>
+      <c r="AF22">
+        <v>240.49999999999901</v>
+      </c>
+      <c r="AG22">
+        <v>240.49999999999901</v>
+      </c>
+      <c r="AH22">
         <v>240.5</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AJ22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="AD23">
+        <v>187.69999999999899</v>
+      </c>
+      <c r="AE23">
+        <v>167.7</v>
+      </c>
+      <c r="AF23">
+        <v>117.30000000000599</v>
+      </c>
+      <c r="AG23">
+        <v>93.5</v>
+      </c>
+      <c r="AH23">
+        <v>123.5</v>
+      </c>
+      <c r="AJ23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA23">
-        <v>187.69999999999899</v>
-      </c>
-      <c r="AB23">
-        <v>167.7</v>
-      </c>
-      <c r="AC23">
-        <v>117.30000000000599</v>
-      </c>
-      <c r="AD23">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD24">
         <v>93.5</v>
       </c>
-      <c r="AE23">
-        <v>123.5</v>
-      </c>
-      <c r="AG23" t="s">
+      <c r="AE24">
+        <v>111</v>
+      </c>
+      <c r="AF24">
+        <v>72.499999563346805</v>
+      </c>
+      <c r="AG24">
+        <v>55.8</v>
+      </c>
+      <c r="AH24">
+        <v>93.5</v>
+      </c>
+      <c r="AJ24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA24">
-        <v>93.5</v>
-      </c>
-      <c r="AB24">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="AD25">
+        <v>73</v>
+      </c>
+      <c r="AE25">
+        <v>80.999999999999901</v>
+      </c>
+      <c r="AF25">
+        <v>40.4</v>
+      </c>
+      <c r="AG25">
+        <v>29.5</v>
+      </c>
+      <c r="AH25">
+        <v>75.5</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD26">
+        <v>49.3</v>
+      </c>
+      <c r="AE26">
+        <v>55.499999999999901</v>
+      </c>
+      <c r="AF26">
+        <v>26</v>
+      </c>
+      <c r="AG26">
+        <v>14.399999999999901</v>
+      </c>
+      <c r="AH26">
+        <v>49.2</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" t="s">
+        <v>41</v>
+      </c>
+      <c r="L27" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="AD27">
+        <v>37.9</v>
+      </c>
+      <c r="AE27">
+        <v>46.8</v>
+      </c>
+      <c r="AF27">
+        <v>16.499999563346801</v>
+      </c>
+      <c r="AG27">
+        <v>3.4999999999999898</v>
+      </c>
+      <c r="AH27">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" t="s">
+        <v>145</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" t="s">
+        <v>57</v>
+      </c>
+      <c r="L29" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>146</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>203</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" t="s">
+        <v>57</v>
+      </c>
+      <c r="K31" t="s">
+        <v>67</v>
+      </c>
+      <c r="L31" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="AG31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" t="s">
+        <v>126</v>
+      </c>
+      <c r="K33" t="s">
+        <v>160</v>
+      </c>
+      <c r="L33" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+      <c r="AG33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
         <v>111</v>
       </c>
-      <c r="AC24">
-        <v>72.499999563346805</v>
-      </c>
-      <c r="AD24">
-        <v>55.8</v>
-      </c>
-      <c r="AE24">
-        <v>93.5</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA25">
-        <v>73</v>
-      </c>
-      <c r="AB25">
-        <v>80.999999999999901</v>
-      </c>
-      <c r="AC25">
-        <v>40.4</v>
-      </c>
-      <c r="AD25">
-        <v>29.5</v>
-      </c>
-      <c r="AE25">
-        <v>75.5</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
+      <c r="E34" t="s">
+        <v>149</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>205</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>127</v>
+      </c>
+      <c r="K35" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
+      <c r="AG35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" t="s">
+        <v>150</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>206</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+      <c r="J37" t="s">
+        <v>128</v>
+      </c>
+      <c r="K37" t="s">
+        <v>161</v>
+      </c>
+      <c r="L37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y37">
+        <v>1</v>
+      </c>
+      <c r="AG37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG38" t="s">
         <v>42</v>
       </c>
-      <c r="D26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA26">
-        <v>49.3</v>
-      </c>
-      <c r="AB26">
-        <v>55.499999999999901</v>
-      </c>
-      <c r="AC26">
-        <v>26</v>
-      </c>
-      <c r="AD26">
-        <v>14.399999999999901</v>
-      </c>
-      <c r="AE26">
-        <v>49.2</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27" t="s">
-        <v>42</v>
-      </c>
-      <c r="K27" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA27">
-        <v>37.9</v>
-      </c>
-      <c r="AB27">
-        <v>46.8</v>
-      </c>
-      <c r="AC27">
-        <v>16.499999563346801</v>
-      </c>
-      <c r="AD27">
-        <v>3.4999999999999898</v>
-      </c>
-      <c r="AE27">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>70</v>
+      </c>
+      <c r="J39" t="s">
+        <v>69</v>
+      </c>
+      <c r="K39" t="s">
+        <v>95</v>
+      </c>
+      <c r="L39" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y39">
+        <v>1</v>
+      </c>
+      <c r="AG39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG40" t="s">
         <v>141</v>
       </c>
-      <c r="E28" t="s">
-        <v>146</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>88</v>
-      </c>
-      <c r="J29" t="s">
-        <v>86</v>
-      </c>
-      <c r="K29" t="s">
-        <v>58</v>
-      </c>
-      <c r="L29" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" t="s">
-        <v>147</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
-        <v>58</v>
-      </c>
-      <c r="J31" t="s">
-        <v>58</v>
-      </c>
-      <c r="K31" t="s">
-        <v>68</v>
-      </c>
-      <c r="L31" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" t="s">
-        <v>149</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>68</v>
-      </c>
-      <c r="J33" t="s">
-        <v>127</v>
-      </c>
-      <c r="K33" t="s">
-        <v>161</v>
-      </c>
-      <c r="L33" t="s">
-        <v>170</v>
-      </c>
-      <c r="AD33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>163</v>
+      </c>
+      <c r="J41" t="s">
+        <v>74</v>
+      </c>
+      <c r="K41" t="s">
+        <v>74</v>
+      </c>
+      <c r="L41" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="AG41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" t="s">
+        <v>153</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>207</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>71</v>
+      </c>
+      <c r="J43" t="s">
         <v>112</v>
       </c>
-      <c r="D34" t="s">
+      <c r="K43" t="s">
+        <v>31</v>
+      </c>
+      <c r="L43" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y43">
+        <v>1</v>
+      </c>
+      <c r="AG43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>154</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>208</v>
+      </c>
+      <c r="AG44" t="s">
         <v>43</v>
       </c>
-      <c r="E34" t="s">
-        <v>150</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
-        <v>69</v>
-      </c>
-      <c r="J35" t="s">
-        <v>128</v>
-      </c>
-      <c r="K35" t="s">
-        <v>61</v>
-      </c>
-      <c r="L35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" t="s">
+        <v>113</v>
+      </c>
+      <c r="K45" t="s">
+        <v>62</v>
+      </c>
+      <c r="L45" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y45">
+        <v>1</v>
+      </c>
+      <c r="AG45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
         <v>112</v>
       </c>
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" t="s">
-        <v>142</v>
-      </c>
-      <c r="E36" t="s">
-        <v>151</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-      <c r="AD36" t="s">
+      <c r="E46" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG46" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>131</v>
+      </c>
+      <c r="J47" t="s">
+        <v>129</v>
+      </c>
+      <c r="K47" t="s">
+        <v>122</v>
+      </c>
+      <c r="L47" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y47">
+        <v>1</v>
+      </c>
+      <c r="AG47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>156</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>209</v>
+      </c>
+      <c r="AG48" t="s">
         <v>70</v>
       </c>
-      <c r="J37" t="s">
-        <v>129</v>
-      </c>
-      <c r="K37" t="s">
-        <v>162</v>
-      </c>
-      <c r="L37" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" t="s">
-        <v>152</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-      <c r="AD38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>71</v>
-      </c>
-      <c r="J39" t="s">
-        <v>70</v>
-      </c>
-      <c r="K39" t="s">
-        <v>96</v>
-      </c>
-      <c r="L39" t="s">
-        <v>174</v>
-      </c>
-      <c r="AD39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" t="s">
-        <v>153</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="AD40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="H41" t="s">
-        <v>164</v>
-      </c>
-      <c r="J41" t="s">
-        <v>75</v>
-      </c>
-      <c r="K41" t="s">
-        <v>75</v>
-      </c>
-      <c r="L41" t="s">
-        <v>175</v>
-      </c>
-      <c r="AD41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" t="s">
-        <v>143</v>
-      </c>
-      <c r="E42" t="s">
-        <v>154</v>
-      </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-      <c r="J42">
-        <v>1</v>
-      </c>
-      <c r="K42">
-        <v>1</v>
-      </c>
-      <c r="L42">
-        <v>1</v>
-      </c>
-      <c r="AD42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="H43" t="s">
-        <v>72</v>
-      </c>
-      <c r="J43" t="s">
-        <v>113</v>
-      </c>
-      <c r="K43" t="s">
-        <v>32</v>
-      </c>
-      <c r="L43" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E44" t="s">
-        <v>155</v>
-      </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="K44">
-        <v>1</v>
-      </c>
-      <c r="L44">
-        <v>1</v>
-      </c>
-      <c r="AD44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="H45" t="s">
-        <v>38</v>
-      </c>
-      <c r="J45" t="s">
-        <v>114</v>
-      </c>
-      <c r="K45" t="s">
-        <v>63</v>
-      </c>
-      <c r="L45" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" t="s">
-        <v>113</v>
-      </c>
-      <c r="E46" t="s">
-        <v>156</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="J46">
-        <v>1</v>
-      </c>
-      <c r="K46">
-        <v>1</v>
-      </c>
-      <c r="L46">
-        <v>1</v>
-      </c>
-      <c r="AD46" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="H47" t="s">
-        <v>132</v>
-      </c>
-      <c r="J47" t="s">
-        <v>130</v>
-      </c>
-      <c r="K47" t="s">
-        <v>123</v>
-      </c>
-      <c r="L47" t="s">
-        <v>177</v>
-      </c>
-      <c r="AD47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E48" t="s">
-        <v>157</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="J48">
-        <v>1</v>
-      </c>
-      <c r="K48">
-        <v>1</v>
-      </c>
-      <c r="L48">
-        <v>1</v>
-      </c>
-      <c r="AD48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -10869,150 +11185,165 @@
         <v>1</v>
       </c>
       <c r="H49" t="s">
+        <v>164</v>
+      </c>
+      <c r="J49" t="s">
+        <v>46</v>
+      </c>
+      <c r="K49" t="s">
+        <v>131</v>
+      </c>
+      <c r="L49" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y49">
+        <v>1</v>
+      </c>
+      <c r="AG49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" t="s">
+        <v>157</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>210</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
         <v>165</v>
       </c>
-      <c r="J49" t="s">
-        <v>47</v>
-      </c>
-      <c r="K49" t="s">
-        <v>132</v>
-      </c>
-      <c r="L49" t="s">
+      <c r="J51" t="s">
+        <v>71</v>
+      </c>
+      <c r="K51" t="s">
+        <v>162</v>
+      </c>
+      <c r="L51" t="s">
         <v>178</v>
       </c>
-      <c r="AD49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="Y51">
+        <v>1</v>
+      </c>
+      <c r="AG51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>120</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>122</v>
       </c>
-      <c r="D50" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D52" t="s">
+        <v>143</v>
+      </c>
+      <c r="E52" t="s">
         <v>158</v>
       </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-      <c r="K50">
-        <v>1</v>
-      </c>
-      <c r="L50">
-        <v>1</v>
-      </c>
-      <c r="AD50" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="H51" t="s">
-        <v>166</v>
-      </c>
-      <c r="J51" t="s">
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
         <v>72</v>
       </c>
-      <c r="K51" t="s">
-        <v>163</v>
-      </c>
-      <c r="L51" t="s">
+      <c r="J53" t="s">
+        <v>130</v>
+      </c>
+      <c r="K53" t="s">
+        <v>63</v>
+      </c>
+      <c r="L53" t="s">
         <v>179</v>
       </c>
-      <c r="AD51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>121</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="Y53">
+        <v>1</v>
+      </c>
+      <c r="AG53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" t="s">
         <v>123</v>
       </c>
-      <c r="D52" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" t="s">
         <v>159</v>
       </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="J52">
-        <v>1</v>
-      </c>
-      <c r="K52">
-        <v>1</v>
-      </c>
-      <c r="L52">
-        <v>1</v>
-      </c>
-      <c r="AD52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
-        <v>73</v>
-      </c>
-      <c r="J53" t="s">
-        <v>131</v>
-      </c>
-      <c r="K53" t="s">
-        <v>64</v>
-      </c>
-      <c r="L53" t="s">
-        <v>180</v>
-      </c>
-      <c r="AD53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>115</v>
-      </c>
-      <c r="B54" t="s">
-        <v>124</v>
-      </c>
-      <c r="D54" t="s">
-        <v>121</v>
-      </c>
-      <c r="E54" t="s">
-        <v>160</v>
-      </c>
       <c r="H54">
         <v>1</v>
       </c>
@@ -11025,11 +11356,14 @@
       <c r="L54">
         <v>1</v>
       </c>
-      <c r="AD54" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Y54" t="s">
+        <v>212</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -11040,24 +11374,27 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J55" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L55" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
+      <c r="AG55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -11068,82 +11405,112 @@
       <c r="L56">
         <v>1</v>
       </c>
-      <c r="AD56" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Y56" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
-      <c r="AD57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD58" t="s">
+      <c r="Y57">
+        <v>1</v>
+      </c>
+      <c r="AG57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Y58" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG58" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Y59">
+        <v>1</v>
+      </c>
+      <c r="AG59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Y60" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Y61">
+        <v>1</v>
+      </c>
+      <c r="AG61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG68" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD60" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD62" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD66" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="67" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD68" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="69" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD69">
+    <row r="69" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG69">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C815582-E8F1-4E30-AA79-22A6929CBCDF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>